<commit_message>
corrected country mapping and improved map description
</commit_message>
<xml_diff>
--- a/data-raw/African_Countries.xlsx
+++ b/data-raw/African_Countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sskorik\Documents\gitrepos\universityrankingafrica\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D153FE86-2CEE-4EA9-A3C3-48FA228B91A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B809C5-8374-4B7D-89E4-9BD1776698B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="201">
   <si>
     <t>University</t>
   </si>
@@ -637,6 +637,15 @@
   </si>
   <si>
     <t>double between 0 and 1</t>
+  </si>
+  <si>
+    <t>The Gambia</t>
+  </si>
+  <si>
+    <t>Côte d'Ivoire</t>
+  </si>
+  <si>
+    <t>Republic of Congo</t>
   </si>
 </sst>
 </file>
@@ -1163,8 +1172,8 @@
   <dimension ref="A1:G999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1669,7 +1678,7 @@
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>198</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>80</v>
@@ -1680,13 +1689,13 @@
       <c r="D21" s="1">
         <v>316</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="3" t="e">
         <f t="array" ref="E21">INDEX('national-gdp-ppp-wb'!$D$2:$D$53,MATCH(Countries!$A21,'national-gdp-ppp-wb'!$A$2:$A$53,0))</f>
-        <v>5481961000</v>
-      </c>
-      <c r="F21" s="3">
+        <v>#N/A</v>
+      </c>
+      <c r="F21" s="3" t="e">
         <f t="array" ref="F21">INDEX('gdp-per-capita-ppp-worldbank'!$D$2:$D$53,MATCH(Countries!$A21,'gdp-per-capita-ppp-worldbank'!$A$2:$A$53,0))</f>
-        <v>2076.5664000000002</v>
+        <v>#N/A</v>
       </c>
       <c r="G21" s="5">
         <v>0.5</v>
@@ -1767,7 +1776,7 @@
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>199</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>80</v>
@@ -1778,13 +1787,13 @@
       <c r="D25" s="1">
         <v>218</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="3" t="e">
         <f t="array" ref="E25">INDEX('national-gdp-ppp-wb'!$D$2:$D$53,MATCH(Countries!$A25,'national-gdp-ppp-wb'!$A$2:$A$53,0))</f>
-        <v>146322500000</v>
-      </c>
-      <c r="F25" s="3">
+        <v>#N/A</v>
+      </c>
+      <c r="F25" s="3" t="e">
         <f t="array" ref="F25">INDEX('gdp-per-capita-ppp-worldbank'!$D$2:$D$53,MATCH(Countries!$A25,'gdp-per-capita-ppp-worldbank'!$A$2:$A$53,0))</f>
-        <v>5325.0303000000004</v>
+        <v>#N/A</v>
       </c>
       <c r="G25" s="5">
         <v>0.55000000000000004</v>
@@ -2142,7 +2151,7 @@
     </row>
     <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>55</v>
+        <v>200</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>81</v>
@@ -2153,13 +2162,13 @@
       <c r="D40" s="1">
         <v>329</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="3" t="e">
         <f t="array" ref="E40">INDEX('national-gdp-ppp-wb'!$D$2:$D$53,MATCH(Countries!$A40,'national-gdp-ppp-wb'!$A$2:$A$53,0))</f>
-        <v>18875290000</v>
-      </c>
-      <c r="F40" s="3">
+        <v>#N/A</v>
+      </c>
+      <c r="F40" s="3" t="e">
         <f t="array" ref="F40">INDEX('gdp-per-capita-ppp-worldbank'!$D$2:$D$53,MATCH(Countries!$A40,'gdp-per-capita-ppp-worldbank'!$A$2:$A$53,0))</f>
-        <v>3234.393</v>
+        <v>#N/A</v>
       </c>
       <c r="G40" s="5">
         <v>0.56999999999999995</v>

</xml_diff>